<commit_message>
all working with lic_2 only (code edited)
</commit_message>
<xml_diff>
--- a/Data/materiales_lic_2.xlsx
+++ b/Data/materiales_lic_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>descripcion</t>
   </si>
@@ -31,55 +31,52 @@
     <t>referencia</t>
   </si>
   <si>
-    <t>Montaje de tubería PE100, ø 25 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 32 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 40 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 50 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 63 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 75 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>Montaje de tubería PE100, ø 90 mm, 1,0 MPa, colocada. Los trabajos incluyen la puesta en obra de la tubería, el tendido y distribución de la misma en las zanjas ejecutadas por TRAGSA, así como la soldadura e identificación de la misma. Los materiales serán suministrados por TRASA en su almacén de obra.</t>
-  </si>
-  <si>
-    <t>unidad suerte m</t>
+    <t>Montaje de tubería PE100, ø 25 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 32 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 40 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 50 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 63 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 75 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>Montaje de tubería PE100, ø 90 mm, 1,0 MPa, colocada</t>
+  </si>
+  <si>
+    <t>109.449</t>
+  </si>
+  <si>
+    <t>92.249</t>
+  </si>
+  <si>
+    <t>67.386</t>
+  </si>
+  <si>
+    <t>67.383</t>
+  </si>
+  <si>
+    <t>32.687</t>
+  </si>
+  <si>
+    <t>12.050</t>
+  </si>
+  <si>
+    <t>7.956</t>
   </si>
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>Página 2, Sección 2.1</t>
-  </si>
-  <si>
-    <t>Nº Uds. 109.449 Ud. m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 92.249 m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 67.386 Ud. m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 67.383 m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 32.687 m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 12.050 m</t>
-  </si>
-  <si>
-    <t>Nº Uds. 7.956 m</t>
+    <t>Pág. 3, apartado 2</t>
   </si>
 </sst>
 </file>
@@ -468,13 +465,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -482,16 +476,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -499,16 +490,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -516,16 +504,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -533,16 +518,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -550,15 +532,12 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -567,16 +546,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>